<commit_message>
Create df for Deman_SpecificDistribution
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10A7550-40F4-499D-87C1-2564B48C3CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926C7138-3CDA-4369-A1C4-79ED6F31B892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -3031,8 +3031,8 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58:A60"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="A39:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4409,8 +4409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE0BB4B-A87E-47DE-8321-0EFAC4350DE2}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5584,7 +5584,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6130,8 +6130,8 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63:B64"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="B58:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7242,8 +7242,8 @@
   <dimension ref="A1:K124"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A124" sqref="A124:K124"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="H26:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -17090,14 +17090,14 @@
   <dimension ref="A1:AI93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" style="6" customWidth="1"/>
     <col min="5" max="35" width="6.42578125" style="7" customWidth="1"/>
@@ -27067,7 +27067,7 @@
   <dimension ref="A1:AI122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
@@ -40146,7 +40146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64963-0CDD-4BE6-B0AC-E6FD0D7CCBEC}">
   <dimension ref="A1:AI122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
     </sheetView>
@@ -53350,7 +53350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465044A0-2557-4FC4-8230-2D5F5E941F36}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Estimate Limits for Biomass
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6593EFC2-E83F-407D-8311-6861052D6340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E16C21-4868-405C-B630-19C824A63E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="382">
   <si>
     <t>tech</t>
   </si>
@@ -1224,6 +1224,12 @@
   <si>
     <t>Steam Turbine -Black Liquor</t>
   </si>
+  <si>
+    <t>BIOMASS_Dummy_Aggregator</t>
+  </si>
+  <si>
+    <t>Dummy technology used to limit biomass capacity</t>
+  </si>
 </sst>
 </file>
 
@@ -2271,7 +2277,7 @@
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2320,6 +2326,9 @@
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2328,13 +2337,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="345">
     <cellStyle name="20% - Accent1" xfId="322" builtinId="30" customBuiltin="1"/>
@@ -2987,11 +2989,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3019,11 +3021,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="26" customFormat="1">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
@@ -3032,7 +3034,7 @@
       <c r="D2" t="s">
         <v>379</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1">
       <c r="A3" t="s">
@@ -3723,6 +3725,20 @@
       </c>
       <c r="D49" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>380</v>
+      </c>
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -4223,18 +4239,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
@@ -5379,11 +5395,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32AD897-F683-4767-9F8A-BBAC538730FF}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5792,6 +5808,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>380</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5800,11 +5830,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C008AD2-9FC6-4B50-8E5B-D9A0AF2799B1}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6697,6 +6727,20 @@
       </c>
       <c r="E52" t="s">
         <v>326</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>380</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -11076,7 +11120,7 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K19" sqref="A16:K19"/>
     </sheetView>
   </sheetViews>
@@ -16556,11 +16600,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CB1107-551A-4401-A108-C4996FB8D590}">
-  <dimension ref="A1:AI66"/>
+  <dimension ref="A1:AI67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -23635,6 +23679,113 @@
         <v>0</v>
       </c>
     </row>
+    <row r="67" spans="1:35">
+      <c r="A67" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="E67" s="20">
+        <v>0</v>
+      </c>
+      <c r="F67" s="20">
+        <v>0</v>
+      </c>
+      <c r="G67" s="20">
+        <v>0</v>
+      </c>
+      <c r="H67" s="20">
+        <v>0</v>
+      </c>
+      <c r="I67" s="20">
+        <v>0</v>
+      </c>
+      <c r="J67" s="20">
+        <v>0</v>
+      </c>
+      <c r="K67" s="20">
+        <v>0</v>
+      </c>
+      <c r="L67" s="20">
+        <v>0</v>
+      </c>
+      <c r="M67" s="20">
+        <v>0</v>
+      </c>
+      <c r="N67" s="20">
+        <v>0</v>
+      </c>
+      <c r="O67" s="20">
+        <v>0</v>
+      </c>
+      <c r="P67" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="20">
+        <v>0</v>
+      </c>
+      <c r="R67" s="20">
+        <v>0</v>
+      </c>
+      <c r="S67" s="20">
+        <v>0</v>
+      </c>
+      <c r="T67" s="20">
+        <v>0</v>
+      </c>
+      <c r="U67" s="20">
+        <v>0</v>
+      </c>
+      <c r="V67" s="20">
+        <v>0</v>
+      </c>
+      <c r="W67" s="20">
+        <v>0</v>
+      </c>
+      <c r="X67" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AG67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI67" s="20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23644,11 +23795,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD5D24F-D6D8-45F0-9B18-7F7BBE5186DB}">
-  <dimension ref="A1:AI91"/>
+  <dimension ref="A1:AI92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92:XFD92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -33398,6 +33549,113 @@
         <v>0</v>
       </c>
     </row>
+    <row r="92" spans="1:35">
+      <c r="A92" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="C92" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="E92" s="20">
+        <v>0</v>
+      </c>
+      <c r="F92" s="20">
+        <v>0</v>
+      </c>
+      <c r="G92" s="20">
+        <v>0</v>
+      </c>
+      <c r="H92" s="20">
+        <v>0</v>
+      </c>
+      <c r="I92" s="20">
+        <v>0</v>
+      </c>
+      <c r="J92" s="20">
+        <v>0</v>
+      </c>
+      <c r="K92" s="20">
+        <v>0</v>
+      </c>
+      <c r="L92" s="20">
+        <v>0</v>
+      </c>
+      <c r="M92" s="20">
+        <v>0</v>
+      </c>
+      <c r="N92" s="20">
+        <v>0</v>
+      </c>
+      <c r="O92" s="20">
+        <v>0</v>
+      </c>
+      <c r="P92" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="20">
+        <v>0</v>
+      </c>
+      <c r="R92" s="20">
+        <v>0</v>
+      </c>
+      <c r="S92" s="20">
+        <v>0</v>
+      </c>
+      <c r="T92" s="20">
+        <v>0</v>
+      </c>
+      <c r="U92" s="20">
+        <v>0</v>
+      </c>
+      <c r="V92" s="20">
+        <v>0</v>
+      </c>
+      <c r="W92" s="20">
+        <v>0</v>
+      </c>
+      <c r="X92" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y92" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AG92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH92" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI92" s="20">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33407,18 +33665,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64963-0CDD-4BE6-B0AC-E6FD0D7CCBEC}">
-  <dimension ref="A1:AI93"/>
+  <dimension ref="A1:AI94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="16" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="12" style="16" customWidth="1"/>
+    <col min="3" max="3" width="15" style="16" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" style="16" customWidth="1"/>
     <col min="5" max="35" width="6.42578125" style="20" customWidth="1"/>
     <col min="36" max="16384" width="9.140625" style="16"/>
@@ -43465,6 +43723,113 @@
         <v>0</v>
       </c>
       <c r="AI93" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:35">
+      <c r="A94" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="E94" s="20">
+        <v>0</v>
+      </c>
+      <c r="F94" s="20">
+        <v>0</v>
+      </c>
+      <c r="G94" s="20">
+        <v>0</v>
+      </c>
+      <c r="H94" s="20">
+        <v>0</v>
+      </c>
+      <c r="I94" s="20">
+        <v>0</v>
+      </c>
+      <c r="J94" s="20">
+        <v>0</v>
+      </c>
+      <c r="K94" s="20">
+        <v>0</v>
+      </c>
+      <c r="L94" s="20">
+        <v>0</v>
+      </c>
+      <c r="M94" s="20">
+        <v>0</v>
+      </c>
+      <c r="N94" s="20">
+        <v>0</v>
+      </c>
+      <c r="O94" s="20">
+        <v>0</v>
+      </c>
+      <c r="P94" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="20">
+        <v>0</v>
+      </c>
+      <c r="R94" s="20">
+        <v>0</v>
+      </c>
+      <c r="S94" s="20">
+        <v>0</v>
+      </c>
+      <c r="T94" s="20">
+        <v>0</v>
+      </c>
+      <c r="U94" s="20">
+        <v>0</v>
+      </c>
+      <c r="V94" s="20">
+        <v>0</v>
+      </c>
+      <c r="W94" s="20">
+        <v>0</v>
+      </c>
+      <c r="X94" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y94" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AC94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AE94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AG94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH94" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI94" s="20">
         <v>0</v>
       </c>
     </row>
@@ -43480,7 +43845,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add Max Capacity for Group of Technologies
</commit_message>
<xml_diff>
--- a/CreateBaseDeck/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateBaseDeck/ExcelUserData/UserDataPart1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateBaseDeck\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD3F3D9-6443-4558-9305-59426C2D5098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7C9515-65F6-45F5-A9E7-4553FD11F450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -3106,8 +3106,8 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:XFD63"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5531,7 +5531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F425B7AA-21D1-411D-A9AF-54EA873F398D}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -17226,9 +17226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CB1107-551A-4401-A108-C4996FB8D590}">
   <dimension ref="A1:AI80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI80" sqref="A80:AI80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -17236,7 +17236,7 @@
     <col min="1" max="1" width="12.5703125" style="16" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" style="16" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="16" customWidth="1"/>
     <col min="5" max="35" width="6.42578125" style="19" customWidth="1"/>
     <col min="36" max="16384" width="9.140625" style="16"/>
   </cols>
@@ -36893,8 +36893,8 @@
   <dimension ref="A1:AI106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107:XFD107"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>